<commit_message>
final version sent to IEEE MC
</commit_message>
<xml_diff>
--- a/QA/OLTC/Figure_1_OLTC.xlsx
+++ b/QA/OLTC/Figure_1_OLTC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\croe\Mortenson\Ahmad Abdullah - Reactive Power Paper\PSSE\OLTC\Pass_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aabdulla\OneDrive - Mortenson\Shared\Reactive Power Paper\GitHubRepo\QA\OLTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CD0D9D-3129-487E-AE84-CE957D3F0A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC7248A-F611-41F2-B17C-E1FAEE79CAD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16080" yWindow="-6210" windowWidth="16080" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure_1" sheetId="1" r:id="rId1"/>
@@ -1473,6 +1473,7 @@
         <c:axId val="707372168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2685,7 +2686,7 @@
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:S5"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,6 +3124,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D3C4D8FB0A1014CB9B02A84EEDBB1C4" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="68abc473beb4d6375e06d88f85b8c53c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f755b192-b9b7-4ca4-ad46-2820fc91761e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b21f5a9a02cc05be7cfadf1c1d423879" ns2:_="">
     <xsd:import namespace="f755b192-b9b7-4ca4-ad46-2820fc91761e"/>
@@ -3254,29 +3270,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32734F84-6E86-48DF-BD31-05EEAB8C0AE6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6E7F6A6-D138-4556-B043-05329A036239}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A83DC5EF-1543-4831-9D48-075FE42646C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A83DC5EF-1543-4831-9D48-075FE42646C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6E7F6A6-D138-4556-B043-05329A036239}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32734F84-6E86-48DF-BD31-05EEAB8C0AE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f755b192-b9b7-4ca4-ad46-2820fc91761e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>